<commit_message>
Changed the project hierarchy
</commit_message>
<xml_diff>
--- a/PCB/Template/BOM Modified.xlsx
+++ b/PCB/Template/BOM Modified.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\AD21\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Adatok\ElektroProjektek\SNES_TST\PCB\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0A3FE2-581C-451D-9ABD-C6141A019014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8428E2-1F44-4CD9-ACCC-76B792F2A28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32685" yWindow="8310" windowWidth="23730" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14550" yWindow="2910" windowWidth="14565" windowHeight="20490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Report" sheetId="1" r:id="rId1"/>
@@ -134,9 +134,6 @@
     <t>Bill of Materials</t>
   </si>
   <si>
-    <t>Column=Vendor</t>
-  </si>
-  <si>
     <t>Column=Manufacturer_Part_Number</t>
   </si>
   <si>
@@ -165,6 +162,9 @@
   </si>
   <si>
     <t>Total Price</t>
+  </si>
+  <si>
+    <t>Column=Manufacturer</t>
   </si>
 </sst>
 </file>
@@ -1018,8 +1018,8 @@
   </sheetPr>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1111,11 +1111,11 @@
     </row>
     <row r="6" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="2"/>
@@ -1128,11 +1128,11 @@
     </row>
     <row r="7" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>
@@ -1181,11 +1181,11 @@
       </c>
       <c r="B10" s="5">
         <f ca="1">TODAY()</f>
-        <v>44496</v>
+        <v>44531</v>
       </c>
       <c r="C10" s="6">
         <f ca="1">NOW()</f>
-        <v>44496.712430208332</v>
+        <v>44531.683448958334</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="2"/>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="12" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="52" t="s">
         <v>4</v>
@@ -1226,22 +1226,22 @@
         <v>2</v>
       </c>
       <c r="F12" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="53" t="s">
-        <v>35</v>
-      </c>
       <c r="H12" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="53" t="s">
-        <v>38</v>
-      </c>
       <c r="J12" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="K12" s="54" t="s">
         <v>43</v>
-      </c>
-      <c r="K12" s="54" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>